<commit_message>
Criando diagrama de classes
</commit_message>
<xml_diff>
--- a/Dicionário de Dados.xlsx
+++ b/Dicionário de Dados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hideki\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\tcc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B26286-52B1-450C-8DB0-D009E4115413}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D5396A-3365-4476-8F26-035CB050505C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="175">
   <si>
     <t>OTIMIZADOR DE BANCO DE DADOS</t>
   </si>
@@ -532,6 +532,21 @@
   </si>
   <si>
     <t>Identificador do objeto</t>
+  </si>
+  <si>
+    <t>file_path</t>
+  </si>
+  <si>
+    <t>varchar(500)</t>
+  </si>
+  <si>
+    <t>Caminho do arquivo</t>
+  </si>
+  <si>
+    <t>file_growth_size_kb</t>
+  </si>
+  <si>
+    <t>Tamanho do fator de crescimento</t>
   </si>
 </sst>
 </file>
@@ -781,41 +796,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -835,16 +815,29 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -855,6 +848,28 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1071,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1011"/>
+  <dimension ref="A1:H1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="G170" sqref="G170"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1102,60 +1117,60 @@
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="22"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="29"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="22"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="29"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="22"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="22"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="29"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1238,14 +1253,14 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="22"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1253,10 +1268,10 @@
       <c r="B12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="22"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="3" t="s">
         <v>26</v>
       </c>
@@ -1271,8 +1286,8 @@
       <c r="B13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="22"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -1280,36 +1295,36 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="22"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="29"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="22"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="29"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1416,14 +1431,14 @@
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="22"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="29"/>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1431,10 +1446,10 @@
       <c r="B23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="22"/>
+      <c r="D23" s="29"/>
       <c r="E23" s="3" t="s">
         <v>26</v>
       </c>
@@ -1449,10 +1464,10 @@
       <c r="B24" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="22"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="8" t="s">
         <v>11</v>
       </c>
@@ -1469,10 +1484,10 @@
       <c r="B25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="22"/>
+      <c r="D25" s="29"/>
       <c r="E25" s="5" t="s">
         <v>31</v>
       </c>
@@ -1484,36 +1499,36 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="22"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="29"/>
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="22"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="29"/>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1614,14 +1629,14 @@
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="22"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="29"/>
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1629,10 +1644,10 @@
       <c r="B35" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="22"/>
+      <c r="D35" s="29"/>
       <c r="E35" s="3" t="s">
         <v>26</v>
       </c>
@@ -1647,8 +1662,8 @@
       <c r="B36" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="33"/>
-      <c r="D36" s="22"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="29"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
@@ -1656,36 +1671,36 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="22"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="29"/>
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="22"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="29"/>
       <c r="H39" s="14"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1788,14 +1803,14 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="22"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="41"/>
+      <c r="G45" s="29"/>
       <c r="H45" s="14"/>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1803,10 +1818,10 @@
       <c r="B46" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C46" s="27" t="s">
+      <c r="C46" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="D46" s="22"/>
+      <c r="D46" s="29"/>
       <c r="E46" s="3" t="s">
         <v>26</v>
       </c>
@@ -1821,10 +1836,10 @@
       <c r="B47" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="C47" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D47" s="22"/>
+      <c r="D47" s="29"/>
       <c r="E47" s="8" t="s">
         <v>11</v>
       </c>
@@ -1840,26 +1855,26 @@
     </row>
     <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
-      <c r="B49" s="23" t="s">
+      <c r="B49" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="22"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="29"/>
       <c r="H49" s="14"/>
     </row>
     <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="13"/>
-      <c r="B50" s="25" t="s">
+      <c r="B50" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="22"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="29"/>
       <c r="H50" s="14"/>
     </row>
     <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1966,14 +1981,14 @@
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
-      <c r="B56" s="26" t="s">
+      <c r="B56" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="24"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24"/>
-      <c r="G56" s="22"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="29"/>
       <c r="H56" s="14"/>
     </row>
     <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1981,10 +1996,10 @@
       <c r="B57" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="27" t="s">
+      <c r="C57" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="D57" s="22"/>
+      <c r="D57" s="29"/>
       <c r="E57" s="3" t="s">
         <v>26</v>
       </c>
@@ -1999,10 +2014,10 @@
       <c r="B58" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C58" s="21" t="s">
+      <c r="C58" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D58" s="22"/>
+      <c r="D58" s="29"/>
       <c r="E58" s="8" t="s">
         <v>51</v>
       </c>
@@ -2017,10 +2032,10 @@
       <c r="B59" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C59" s="21" t="s">
+      <c r="C59" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D59" s="22"/>
+      <c r="D59" s="29"/>
       <c r="E59" s="5" t="s">
         <v>31</v>
       </c>
@@ -2036,26 +2051,26 @@
     </row>
     <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
-      <c r="B61" s="23" t="s">
+      <c r="B61" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24"/>
-      <c r="F61" s="24"/>
-      <c r="G61" s="22"/>
+      <c r="C61" s="41"/>
+      <c r="D61" s="41"/>
+      <c r="E61" s="41"/>
+      <c r="F61" s="41"/>
+      <c r="G61" s="29"/>
       <c r="H61" s="14"/>
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
-      <c r="B62" s="25" t="s">
+      <c r="B62" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
-      <c r="G62" s="22"/>
+      <c r="C62" s="41"/>
+      <c r="D62" s="41"/>
+      <c r="E62" s="41"/>
+      <c r="F62" s="41"/>
+      <c r="G62" s="29"/>
       <c r="H62" s="14"/>
     </row>
     <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2144,7 +2159,7 @@
       <c r="C67" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="D67" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E67" s="7"/>
@@ -2158,1762 +2173,1813 @@
     </row>
     <row r="68" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
-      <c r="B68" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="24"/>
-      <c r="F68" s="24"/>
-      <c r="G68" s="22"/>
+      <c r="B68" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68" s="7"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="H68" s="14"/>
     </row>
     <row r="69" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
-      <c r="B69" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C69" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D69" s="22"/>
-      <c r="E69" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G69" s="3"/>
+      <c r="B69" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C69" s="41"/>
+      <c r="D69" s="41"/>
+      <c r="E69" s="41"/>
+      <c r="F69" s="41"/>
+      <c r="G69" s="29"/>
       <c r="H69" s="14"/>
     </row>
     <row r="70" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
-      <c r="B70" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C70" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D70" s="22"/>
-      <c r="E70" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G70" s="10"/>
+      <c r="B70" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D70" s="29"/>
+      <c r="E70" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G70" s="3"/>
       <c r="H70" s="14"/>
     </row>
     <row r="71" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
+      <c r="B71" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D71" s="29"/>
+      <c r="E71" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G71" s="10"/>
       <c r="H71" s="14"/>
     </row>
     <row r="72" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
-      <c r="B72" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C72" s="24"/>
-      <c r="D72" s="24"/>
-      <c r="E72" s="24"/>
-      <c r="F72" s="24"/>
-      <c r="G72" s="22"/>
       <c r="H72" s="14"/>
     </row>
     <row r="73" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
-      <c r="B73" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C73" s="24"/>
-      <c r="D73" s="24"/>
-      <c r="E73" s="24"/>
-      <c r="F73" s="24"/>
-      <c r="G73" s="22"/>
+      <c r="B73" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C73" s="41"/>
+      <c r="D73" s="41"/>
+      <c r="E73" s="41"/>
+      <c r="F73" s="41"/>
+      <c r="G73" s="29"/>
       <c r="H73" s="14"/>
     </row>
     <row r="74" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="13"/>
-      <c r="B74" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="B74" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C74" s="41"/>
+      <c r="D74" s="41"/>
+      <c r="E74" s="41"/>
+      <c r="F74" s="41"/>
+      <c r="G74" s="29"/>
       <c r="H74" s="14"/>
     </row>
     <row r="75" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="13"/>
-      <c r="B75" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D75" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E75" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F75" s="7"/>
-      <c r="G75" s="8" t="s">
-        <v>74</v>
+      <c r="B75" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H75" s="14"/>
     </row>
     <row r="76" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="13"/>
       <c r="B76" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E76" s="11"/>
+        <v>73</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="F76" s="7"/>
       <c r="G76" s="8" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="H76" s="14"/>
     </row>
     <row r="77" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="13"/>
       <c r="B77" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E77" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="E77" s="11"/>
       <c r="F77" s="7"/>
       <c r="G77" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H77" s="14"/>
     </row>
     <row r="78" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
-      <c r="B78" s="16" t="s">
-        <v>35</v>
+      <c r="B78" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>12</v>
+        <v>68</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="E78" s="7"/>
-      <c r="F78" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="F78" s="7"/>
       <c r="G78" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H78" s="14"/>
     </row>
     <row r="79" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="13"/>
       <c r="B79" s="16" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>21</v>
+        <v>58</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="E79" s="7"/>
-      <c r="F79" s="7"/>
+      <c r="F79" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="G79" s="8" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="H79" s="14"/>
     </row>
     <row r="80" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="13"/>
-      <c r="B80" s="11">
-        <v>6</v>
+      <c r="B80" s="16" t="s">
+        <v>50</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E80" s="11"/>
-      <c r="F80" s="11" t="s">
-        <v>13</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
       <c r="G80" s="8" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="H80" s="14"/>
     </row>
     <row r="81" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="13"/>
-      <c r="B81" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="24"/>
-      <c r="G81" s="22"/>
+      <c r="B81" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G81" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="H81" s="14"/>
     </row>
     <row r="82" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="13"/>
-      <c r="B82" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C82" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D82" s="22"/>
-      <c r="E82" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G82" s="3"/>
+      <c r="B82" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="8" t="s">
+        <v>172</v>
+      </c>
       <c r="H82" s="14"/>
     </row>
     <row r="83" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13"/>
       <c r="B83" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C83" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D83" s="22"/>
-      <c r="E83" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F83" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G83" s="10"/>
+        <v>88</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="8" t="s">
+        <v>174</v>
+      </c>
       <c r="H83" s="14"/>
     </row>
     <row r="84" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="13"/>
-      <c r="B84" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C84" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="D84" s="22"/>
-      <c r="E84" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G84" s="10"/>
+      <c r="B84" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C84" s="41"/>
+      <c r="D84" s="41"/>
+      <c r="E84" s="41"/>
+      <c r="F84" s="41"/>
+      <c r="G84" s="29"/>
       <c r="H84" s="14"/>
     </row>
     <row r="85" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13"/>
-      <c r="G85" s="34"/>
+      <c r="B85" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C85" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D85" s="29"/>
+      <c r="E85" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G85" s="3"/>
       <c r="H85" s="14"/>
     </row>
     <row r="86" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="13"/>
-      <c r="B86" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="C86" s="24"/>
-      <c r="D86" s="24"/>
-      <c r="E86" s="24"/>
-      <c r="F86" s="24"/>
-      <c r="G86" s="22"/>
+      <c r="B86" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C86" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D86" s="29"/>
+      <c r="E86" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F86" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G86" s="10"/>
       <c r="H86" s="14"/>
     </row>
     <row r="87" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="13"/>
-      <c r="B87" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C87" s="24"/>
-      <c r="D87" s="24"/>
-      <c r="E87" s="24"/>
-      <c r="F87" s="24"/>
-      <c r="G87" s="22"/>
+      <c r="B87" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D87" s="29"/>
+      <c r="E87" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G87" s="10"/>
       <c r="H87" s="14"/>
     </row>
     <row r="88" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="13"/>
-      <c r="B88" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="G88" s="21"/>
       <c r="H88" s="14"/>
     </row>
     <row r="89" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="13"/>
-      <c r="B89" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C89" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D89" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E89" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="F89" s="11"/>
-      <c r="G89" s="8" t="s">
-        <v>87</v>
-      </c>
+      <c r="B89" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C89" s="41"/>
+      <c r="D89" s="41"/>
+      <c r="E89" s="41"/>
+      <c r="F89" s="41"/>
+      <c r="G89" s="29"/>
       <c r="H89" s="14"/>
     </row>
     <row r="90" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="13"/>
-      <c r="B90" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C90" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="D90" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E90" s="35"/>
-      <c r="F90" s="11"/>
-      <c r="G90" s="38" t="s">
-        <v>169</v>
-      </c>
+      <c r="B90" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C90" s="41"/>
+      <c r="D90" s="41"/>
+      <c r="E90" s="41"/>
+      <c r="F90" s="41"/>
+      <c r="G90" s="29"/>
       <c r="H90" s="14"/>
     </row>
     <row r="91" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="13"/>
-      <c r="B91" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D91" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E91" s="11"/>
-      <c r="F91" s="7"/>
-      <c r="G91" s="8" t="s">
-        <v>80</v>
+      <c r="B91" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H91" s="14"/>
     </row>
     <row r="92" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="13"/>
-      <c r="B92" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="C92" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="D92" s="8" t="s">
+      <c r="B92" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D92" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E92" s="7"/>
-      <c r="F92" s="11" t="s">
+      <c r="E92" s="22" t="s">
         <v>13</v>
       </c>
+      <c r="F92" s="11"/>
       <c r="G92" s="8" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="H92" s="14"/>
     </row>
     <row r="93" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
-      <c r="B93" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D93" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E93" s="7"/>
+      <c r="B93" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C93" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="D93" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E93" s="22"/>
       <c r="F93" s="11"/>
-      <c r="G93" s="8" t="s">
-        <v>83</v>
+      <c r="G93" s="25" t="s">
+        <v>169</v>
       </c>
       <c r="H93" s="14"/>
     </row>
     <row r="94" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="13"/>
-      <c r="B94" s="39" t="s">
-        <v>72</v>
+      <c r="B94" s="23" t="s">
+        <v>19</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E94" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="E94" s="11"/>
       <c r="F94" s="7"/>
       <c r="G94" s="8" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="H94" s="14"/>
     </row>
     <row r="95" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="13"/>
-      <c r="B95" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>20</v>
+      <c r="B95" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C95" s="24" t="s">
+        <v>58</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="E95" s="7"/>
-      <c r="F95" s="7"/>
+      <c r="F95" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="G95" s="8" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="H95" s="14"/>
     </row>
     <row r="96" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="13"/>
-      <c r="B96" s="39" t="s">
-        <v>88</v>
+      <c r="B96" s="26" t="s">
+        <v>50</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D96" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E96" s="11"/>
-      <c r="F96" s="11" t="s">
-        <v>13</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E96" s="7"/>
+      <c r="F96" s="11"/>
       <c r="G96" s="8" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="H96" s="14"/>
     </row>
     <row r="97" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="13"/>
       <c r="B97" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C97" s="24"/>
-      <c r="D97" s="24"/>
-      <c r="E97" s="24"/>
-      <c r="F97" s="24"/>
-      <c r="G97" s="22"/>
+        <v>72</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7"/>
+      <c r="G97" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="H97" s="14"/>
     </row>
     <row r="98" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="13"/>
-      <c r="B98" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C98" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D98" s="22"/>
-      <c r="E98" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F98" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G98" s="3"/>
+      <c r="B98" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E98" s="7"/>
+      <c r="F98" s="7"/>
+      <c r="G98" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="H98" s="14"/>
     </row>
     <row r="99" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="13"/>
-      <c r="B99" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C99" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D99" s="22"/>
-      <c r="E99" s="8" t="s">
+      <c r="B99" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C99" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F99" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G99" s="10"/>
+      <c r="D99" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E99" s="11"/>
+      <c r="F99" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G99" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="H99" s="14"/>
     </row>
     <row r="100" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13"/>
-      <c r="B100" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C100" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="D100" s="22"/>
-      <c r="E100" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="F100" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="G100" s="10"/>
+      <c r="B100" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C100" s="41"/>
+      <c r="D100" s="41"/>
+      <c r="E100" s="41"/>
+      <c r="F100" s="41"/>
+      <c r="G100" s="29"/>
       <c r="H100" s="14"/>
     </row>
     <row r="101" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
+      <c r="B101" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C101" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D101" s="29"/>
+      <c r="E101" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G101" s="3"/>
       <c r="H101" s="14"/>
     </row>
     <row r="102" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="13"/>
-      <c r="B102" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="C102" s="24"/>
-      <c r="D102" s="24"/>
-      <c r="E102" s="24"/>
-      <c r="F102" s="24"/>
-      <c r="G102" s="22"/>
+      <c r="B102" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D102" s="29"/>
+      <c r="E102" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F102" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G102" s="10"/>
       <c r="H102" s="14"/>
     </row>
     <row r="103" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="13"/>
-      <c r="B103" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="C103" s="24"/>
-      <c r="D103" s="24"/>
-      <c r="E103" s="24"/>
-      <c r="F103" s="24"/>
-      <c r="G103" s="22"/>
+      <c r="B103" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C103" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D103" s="29"/>
+      <c r="E103" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F103" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="G103" s="10"/>
       <c r="H103" s="14"/>
     </row>
     <row r="104" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="13"/>
-      <c r="B104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G104" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="H104" s="14"/>
     </row>
     <row r="105" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="13"/>
-      <c r="B105" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C105" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="D105" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E105" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F105" s="11"/>
-      <c r="G105" s="17" t="s">
-        <v>92</v>
-      </c>
+      <c r="B105" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C105" s="41"/>
+      <c r="D105" s="41"/>
+      <c r="E105" s="41"/>
+      <c r="F105" s="41"/>
+      <c r="G105" s="29"/>
       <c r="H105" s="14"/>
     </row>
     <row r="106" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="13"/>
-      <c r="B106" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C106" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="D106" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E106" s="11"/>
-      <c r="F106" s="11"/>
-      <c r="G106" s="17" t="s">
-        <v>94</v>
-      </c>
+      <c r="B106" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C106" s="41"/>
+      <c r="D106" s="41"/>
+      <c r="E106" s="41"/>
+      <c r="F106" s="41"/>
+      <c r="G106" s="29"/>
       <c r="H106" s="14"/>
     </row>
     <row r="107" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="13"/>
-      <c r="B107" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C107" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D107" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E107" s="11"/>
-      <c r="F107" s="11"/>
-      <c r="G107" s="17" t="s">
-        <v>22</v>
+      <c r="B107" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H107" s="14"/>
     </row>
     <row r="108" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="13"/>
-      <c r="B108" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C108" s="17" t="s">
-        <v>81</v>
+      <c r="B108" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C108" s="27" t="s">
+        <v>120</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E108" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="F108" s="11"/>
       <c r="G108" s="17" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="H108" s="14"/>
     </row>
     <row r="109" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="13"/>
-      <c r="B109" s="16" t="s">
-        <v>50</v>
+      <c r="B109" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C109" s="17" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="E109" s="11"/>
       <c r="F109" s="11"/>
       <c r="G109" s="17" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="H109" s="14"/>
     </row>
     <row r="110" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="13"/>
-      <c r="B110" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C110" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="D110" s="6" t="s">
-        <v>12</v>
+      <c r="B110" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C110" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="E110" s="11"/>
-      <c r="F110" s="35" t="s">
-        <v>13</v>
-      </c>
+      <c r="F110" s="11"/>
       <c r="G110" s="17" t="s">
-        <v>97</v>
+        <v>22</v>
       </c>
       <c r="H110" s="14"/>
     </row>
     <row r="111" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="13"/>
-      <c r="B111" s="11" t="s">
-        <v>75</v>
+      <c r="B111" s="16" t="s">
+        <v>35</v>
       </c>
       <c r="C111" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="D111" s="6" t="s">
-        <v>12</v>
+        <v>81</v>
+      </c>
+      <c r="D111" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="E111" s="11"/>
-      <c r="F111" s="35" t="s">
-        <v>13</v>
-      </c>
+      <c r="F111" s="11"/>
       <c r="G111" s="17" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="H111" s="14"/>
     </row>
     <row r="112" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="13"/>
-      <c r="B112" s="11" t="s">
-        <v>88</v>
+      <c r="B112" s="16" t="s">
+        <v>50</v>
       </c>
       <c r="C112" s="17" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="E112" s="11"/>
       <c r="F112" s="11"/>
       <c r="G112" s="17" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="H112" s="14"/>
     </row>
     <row r="113" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="13"/>
       <c r="B113" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C113" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="D113" s="8" t="s">
-        <v>104</v>
+        <v>72</v>
+      </c>
+      <c r="C113" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="E113" s="11"/>
-      <c r="F113" s="11"/>
+      <c r="F113" s="22" t="s">
+        <v>13</v>
+      </c>
       <c r="G113" s="17" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="H113" s="14"/>
     </row>
     <row r="114" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="13"/>
       <c r="B114" s="11" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C114" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="D114" s="8" t="s">
-        <v>104</v>
+        <v>98</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="E114" s="11"/>
-      <c r="F114" s="11"/>
+      <c r="F114" s="22" t="s">
+        <v>13</v>
+      </c>
       <c r="G114" s="17" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="H114" s="14"/>
     </row>
     <row r="115" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="13"/>
       <c r="B115" s="11" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="C115" s="17" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>104</v>
+        <v>17</v>
       </c>
       <c r="E115" s="11"/>
       <c r="F115" s="11"/>
       <c r="G115" s="17" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="H115" s="14"/>
     </row>
     <row r="116" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="13"/>
       <c r="B116" s="11" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C116" s="17" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E116" s="11"/>
       <c r="F116" s="11"/>
       <c r="G116" s="17" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="H116" s="14"/>
     </row>
     <row r="117" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="13"/>
       <c r="B117" s="11" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C117" s="17" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E117" s="11"/>
       <c r="F117" s="11"/>
       <c r="G117" s="17" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="H117" s="14"/>
     </row>
     <row r="118" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="13"/>
       <c r="B118" s="11" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C118" s="17" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E118" s="11"/>
       <c r="F118" s="11"/>
       <c r="G118" s="17" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="H118" s="14"/>
     </row>
     <row r="119" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="14"/>
+      <c r="A119" s="13"/>
       <c r="B119" s="11" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C119" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D119" s="10" t="s">
-        <v>12</v>
+        <v>113</v>
+      </c>
+      <c r="D119" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="E119" s="11"/>
-      <c r="F119" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G119" s="40" t="s">
-        <v>52</v>
+      <c r="F119" s="11"/>
+      <c r="G119" s="17" t="s">
+        <v>115</v>
       </c>
       <c r="H119" s="14"/>
     </row>
     <row r="120" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="13"/>
-      <c r="B120" s="11">
-        <v>16</v>
-      </c>
-      <c r="C120" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="D120" s="6" t="s">
-        <v>12</v>
+      <c r="B120" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C120" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D120" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="E120" s="11"/>
       <c r="F120" s="11"/>
-      <c r="G120" s="40" t="s">
-        <v>169</v>
+      <c r="G120" s="17" t="s">
+        <v>118</v>
       </c>
       <c r="H120" s="14"/>
     </row>
     <row r="121" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="13"/>
-      <c r="B121" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C121" s="24"/>
-      <c r="D121" s="24"/>
-      <c r="E121" s="24"/>
-      <c r="F121" s="24"/>
-      <c r="G121" s="22"/>
+      <c r="B121" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C121" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D121" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E121" s="11"/>
+      <c r="F121" s="11"/>
+      <c r="G121" s="17" t="s">
+        <v>121</v>
+      </c>
       <c r="H121" s="14"/>
     </row>
     <row r="122" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="13"/>
-      <c r="B122" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C122" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D122" s="22"/>
-      <c r="E122" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F122" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G122" s="3"/>
+      <c r="A122" s="14"/>
+      <c r="B122" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C122" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D122" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E122" s="11"/>
+      <c r="F122" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G122" s="27" t="s">
+        <v>52</v>
+      </c>
       <c r="H122" s="14"/>
     </row>
     <row r="123" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="13"/>
-      <c r="B123" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C123" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D123" s="22"/>
-      <c r="E123" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F123" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G123" s="10"/>
+      <c r="B123" s="11">
+        <v>16</v>
+      </c>
+      <c r="C123" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E123" s="11"/>
+      <c r="F123" s="11"/>
+      <c r="G123" s="27" t="s">
+        <v>169</v>
+      </c>
       <c r="H123" s="14"/>
     </row>
     <row r="124" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="13"/>
-      <c r="B124" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C124" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="D124" s="22"/>
-      <c r="E124" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="F124" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="G124" s="10"/>
+      <c r="B124" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C124" s="41"/>
+      <c r="D124" s="41"/>
+      <c r="E124" s="41"/>
+      <c r="F124" s="41"/>
+      <c r="G124" s="29"/>
       <c r="H124" s="14"/>
     </row>
     <row r="125" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="13"/>
-      <c r="B125" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="C125" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="D125" s="22"/>
-      <c r="E125" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="F125" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="G125" s="10"/>
+      <c r="B125" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C125" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D125" s="29"/>
+      <c r="E125" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G125" s="3"/>
       <c r="H125" s="14"/>
     </row>
     <row r="126" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="13"/>
+      <c r="B126" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C126" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D126" s="29"/>
+      <c r="E126" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F126" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G126" s="10"/>
       <c r="H126" s="14"/>
     </row>
     <row r="127" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="13"/>
-      <c r="B127" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="C127" s="45"/>
-      <c r="D127" s="45"/>
-      <c r="E127" s="45"/>
-      <c r="F127" s="45"/>
-      <c r="G127" s="46"/>
+      <c r="B127" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C127" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="D127" s="29"/>
+      <c r="E127" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F127" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G127" s="10"/>
       <c r="H127" s="14"/>
     </row>
     <row r="128" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="13"/>
-      <c r="B128" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="C128" s="43"/>
-      <c r="D128" s="43"/>
-      <c r="E128" s="43"/>
-      <c r="F128" s="43"/>
-      <c r="G128" s="44"/>
+      <c r="B128" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C128" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="D128" s="29"/>
+      <c r="E128" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F128" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G128" s="10"/>
       <c r="H128" s="14"/>
     </row>
     <row r="129" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="13"/>
-      <c r="B129" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D129" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E129" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F129" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G129" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="H129" s="14"/>
     </row>
     <row r="130" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="13"/>
-      <c r="B130" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C130" s="40" t="s">
-        <v>133</v>
-      </c>
-      <c r="D130" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E130" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F130" s="11"/>
-      <c r="G130" s="17" t="s">
-        <v>125</v>
-      </c>
+      <c r="B130" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="C130" s="37"/>
+      <c r="D130" s="37"/>
+      <c r="E130" s="37"/>
+      <c r="F130" s="37"/>
+      <c r="G130" s="38"/>
       <c r="H130" s="14"/>
     </row>
     <row r="131" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="13"/>
-      <c r="B131" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C131" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="D131" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E131" s="11"/>
-      <c r="F131" s="11"/>
-      <c r="G131" s="17" t="s">
-        <v>127</v>
-      </c>
+      <c r="B131" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C131" s="34"/>
+      <c r="D131" s="34"/>
+      <c r="E131" s="34"/>
+      <c r="F131" s="34"/>
+      <c r="G131" s="35"/>
       <c r="H131" s="14"/>
     </row>
     <row r="132" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="13"/>
-      <c r="B132" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C132" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D132" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E132" s="11"/>
-      <c r="F132" s="11"/>
-      <c r="G132" s="17" t="s">
-        <v>22</v>
+      <c r="B132" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H132" s="14"/>
     </row>
     <row r="133" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="13"/>
-      <c r="B133" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C133" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D133" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E133" s="11"/>
+      <c r="B133" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C133" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="D133" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E133" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="F133" s="11"/>
       <c r="G133" s="17" t="s">
-        <v>83</v>
+        <v>125</v>
       </c>
       <c r="H133" s="14"/>
     </row>
     <row r="134" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="13"/>
-      <c r="B134" s="16" t="s">
-        <v>50</v>
+      <c r="B134" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C134" s="17" t="s">
-        <v>84</v>
+        <v>126</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="E134" s="11"/>
       <c r="F134" s="11"/>
       <c r="G134" s="17" t="s">
-        <v>6</v>
+        <v>127</v>
       </c>
       <c r="H134" s="14"/>
     </row>
     <row r="135" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="13"/>
-      <c r="B135" s="11" t="s">
-        <v>72</v>
+      <c r="B135" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C135" s="17" t="s">
-        <v>128</v>
+        <v>20</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E135" s="11"/>
       <c r="F135" s="11"/>
       <c r="G135" s="17" t="s">
-        <v>129</v>
+        <v>22</v>
       </c>
       <c r="H135" s="14"/>
     </row>
     <row r="136" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="13"/>
-      <c r="B136" s="11" t="s">
-        <v>75</v>
+      <c r="B136" s="16" t="s">
+        <v>35</v>
       </c>
       <c r="C136" s="17" t="s">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E136" s="11"/>
       <c r="F136" s="11"/>
       <c r="G136" s="17" t="s">
-        <v>131</v>
+        <v>83</v>
       </c>
       <c r="H136" s="14"/>
     </row>
     <row r="137" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="13"/>
-      <c r="B137" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C137" s="40" t="s">
-        <v>86</v>
+      <c r="B137" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C137" s="17" t="s">
+        <v>84</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>132</v>
+        <v>85</v>
       </c>
       <c r="E137" s="11"/>
-      <c r="F137" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="F137" s="11"/>
       <c r="G137" s="17" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="H137" s="14"/>
     </row>
     <row r="138" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="13"/>
       <c r="B138" s="11" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="C138" s="17" t="s">
-        <v>51</v>
+        <v>128</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="E138" s="11"/>
-      <c r="F138" s="35" t="s">
-        <v>13</v>
-      </c>
+      <c r="F138" s="11"/>
       <c r="G138" s="17" t="s">
-        <v>52</v>
+        <v>129</v>
       </c>
       <c r="H138" s="14"/>
     </row>
     <row r="139" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="13"/>
       <c r="B139" s="11" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="C139" s="17" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="E139" s="11"/>
       <c r="F139" s="11"/>
       <c r="G139" s="17" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H139" s="14"/>
     </row>
     <row r="140" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="13"/>
-      <c r="B140" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C140" s="41"/>
-      <c r="D140" s="41"/>
-      <c r="E140" s="41"/>
-      <c r="F140" s="41"/>
-      <c r="G140" s="42"/>
+      <c r="B140" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C140" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D140" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E140" s="11"/>
+      <c r="F140" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G140" s="17" t="s">
+        <v>78</v>
+      </c>
       <c r="H140" s="14"/>
     </row>
     <row r="141" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="13"/>
-      <c r="B141" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C141" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D141" s="22"/>
-      <c r="E141" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F141" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G141" s="3"/>
+      <c r="B141" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C141" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D141" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E141" s="11"/>
+      <c r="F141" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G141" s="17" t="s">
+        <v>52</v>
+      </c>
       <c r="H141" s="14"/>
     </row>
     <row r="142" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="13"/>
-      <c r="B142" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C142" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D142" s="22"/>
-      <c r="E142" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F142" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G142" s="10"/>
+      <c r="B142" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C142" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D142" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E142" s="11"/>
+      <c r="F142" s="11"/>
+      <c r="G142" s="17" t="s">
+        <v>136</v>
+      </c>
       <c r="H142" s="14"/>
     </row>
     <row r="143" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="13"/>
-      <c r="B143" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C143" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="D143" s="22"/>
-      <c r="E143" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="F143" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="G143" s="10"/>
+      <c r="B143" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C143" s="31"/>
+      <c r="D143" s="31"/>
+      <c r="E143" s="31"/>
+      <c r="F143" s="31"/>
+      <c r="G143" s="32"/>
       <c r="H143" s="14"/>
     </row>
     <row r="144" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="13"/>
+      <c r="B144" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C144" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D144" s="29"/>
+      <c r="E144" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F144" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G144" s="3"/>
       <c r="H144" s="14"/>
     </row>
     <row r="145" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="13"/>
-      <c r="B145" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="C145" s="45"/>
-      <c r="D145" s="45"/>
-      <c r="E145" s="45"/>
-      <c r="F145" s="45"/>
-      <c r="G145" s="46"/>
+      <c r="B145" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C145" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D145" s="29"/>
+      <c r="E145" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F145" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G145" s="10"/>
       <c r="H145" s="14"/>
     </row>
     <row r="146" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="13"/>
-      <c r="B146" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="C146" s="43"/>
-      <c r="D146" s="43"/>
-      <c r="E146" s="43"/>
-      <c r="F146" s="43"/>
-      <c r="G146" s="44"/>
+      <c r="B146" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C146" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D146" s="29"/>
+      <c r="E146" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="F146" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G146" s="10"/>
       <c r="H146" s="14"/>
     </row>
     <row r="147" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="13"/>
-      <c r="B147" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D147" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E147" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F147" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G147" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="H147" s="14"/>
     </row>
     <row r="148" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="13"/>
-      <c r="B148" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C148" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="D148" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E148" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F148" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G148" s="17" t="s">
-        <v>78</v>
-      </c>
+      <c r="B148" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="C148" s="37"/>
+      <c r="D148" s="37"/>
+      <c r="E148" s="37"/>
+      <c r="F148" s="37"/>
+      <c r="G148" s="38"/>
       <c r="H148" s="14"/>
     </row>
     <row r="149" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="13"/>
-      <c r="B149" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C149" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="D149" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E149" s="11"/>
-      <c r="F149" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G149" s="17" t="s">
-        <v>71</v>
-      </c>
+      <c r="B149" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="C149" s="34"/>
+      <c r="D149" s="34"/>
+      <c r="E149" s="34"/>
+      <c r="F149" s="34"/>
+      <c r="G149" s="35"/>
       <c r="H149" s="14"/>
     </row>
     <row r="150" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="13"/>
-      <c r="B150" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C150" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="D150" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E150" s="18"/>
-      <c r="F150" s="11"/>
-      <c r="G150" s="17" t="s">
-        <v>141</v>
+      <c r="B150" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H150" s="14"/>
     </row>
     <row r="151" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="13"/>
-      <c r="B151" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C151" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D151" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E151" s="11"/>
-      <c r="F151" s="11"/>
+      <c r="B151" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C151" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D151" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E151" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F151" s="18" t="s">
+        <v>13</v>
+      </c>
       <c r="G151" s="17" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H151" s="14"/>
     </row>
     <row r="152" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="13"/>
-      <c r="B152" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C152" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D152" s="8" t="s">
-        <v>95</v>
+      <c r="B152" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C152" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D152" s="19" t="s">
+        <v>12</v>
       </c>
       <c r="E152" s="11"/>
-      <c r="F152" s="11"/>
+      <c r="F152" s="18" t="s">
+        <v>13</v>
+      </c>
       <c r="G152" s="17" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="H152" s="14"/>
     </row>
     <row r="153" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="13"/>
-      <c r="B153" s="11" t="s">
-        <v>72</v>
+      <c r="B153" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C153" s="17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E153" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="E153" s="18"/>
       <c r="F153" s="11"/>
       <c r="G153" s="17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H153" s="14"/>
     </row>
     <row r="154" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="13"/>
-      <c r="B154" s="11" t="s">
-        <v>75</v>
+      <c r="B154" s="16" t="s">
+        <v>35</v>
       </c>
       <c r="C154" s="17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D154" s="8" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E154" s="11"/>
       <c r="F154" s="11"/>
       <c r="G154" s="17" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="H154" s="14"/>
     </row>
     <row r="155" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="13"/>
-      <c r="B155" s="11" t="s">
-        <v>88</v>
+      <c r="B155" s="16" t="s">
+        <v>50</v>
       </c>
       <c r="C155" s="17" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="D155" s="8" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="E155" s="11"/>
       <c r="F155" s="11"/>
       <c r="G155" s="17" t="s">
-        <v>146</v>
+        <v>22</v>
       </c>
       <c r="H155" s="14"/>
     </row>
     <row r="156" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="13"/>
       <c r="B156" s="11" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="C156" s="17" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D156" s="8" t="s">
-        <v>145</v>
+        <v>17</v>
       </c>
       <c r="E156" s="11"/>
       <c r="F156" s="11"/>
       <c r="G156" s="17" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H156" s="14"/>
     </row>
     <row r="157" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="13"/>
       <c r="B157" s="11" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C157" s="17" t="s">
-        <v>149</v>
+        <v>84</v>
       </c>
       <c r="D157" s="8" t="s">
-        <v>132</v>
+        <v>85</v>
       </c>
       <c r="E157" s="11"/>
       <c r="F157" s="11"/>
       <c r="G157" s="17" t="s">
-        <v>150</v>
+        <v>6</v>
       </c>
       <c r="H157" s="14"/>
     </row>
     <row r="158" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="13"/>
       <c r="B158" s="11" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="C158" s="17" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="E158" s="11"/>
       <c r="F158" s="11"/>
       <c r="G158" s="17" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="H158" s="14"/>
     </row>
     <row r="159" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="13"/>
       <c r="B159" s="11" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C159" s="17" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D159" s="8" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="E159" s="11"/>
       <c r="F159" s="11"/>
       <c r="G159" s="17" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="H159" s="14"/>
     </row>
     <row r="160" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="13"/>
       <c r="B160" s="11" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C160" s="17" t="s">
-        <v>113</v>
+        <v>149</v>
       </c>
       <c r="D160" s="8" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="E160" s="11"/>
       <c r="F160" s="11"/>
       <c r="G160" s="17" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H160" s="14"/>
     </row>
     <row r="161" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="13"/>
       <c r="B161" s="11" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C161" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="D161" s="19" t="s">
-        <v>157</v>
+        <v>151</v>
+      </c>
+      <c r="D161" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="E161" s="11"/>
       <c r="F161" s="11"/>
       <c r="G161" s="17" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="H161" s="14"/>
     </row>
     <row r="162" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="13"/>
       <c r="B162" s="11" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C162" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="D162" s="19" t="s">
-        <v>145</v>
+        <v>153</v>
+      </c>
+      <c r="D162" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="E162" s="11"/>
       <c r="F162" s="11"/>
       <c r="G162" s="17" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="H162" s="14"/>
     </row>
     <row r="163" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="13"/>
       <c r="B163" s="11" t="s">
-        <v>161</v>
+        <v>116</v>
       </c>
       <c r="C163" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="D163" s="19" t="s">
-        <v>145</v>
+        <v>113</v>
+      </c>
+      <c r="D163" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="E163" s="11"/>
       <c r="F163" s="11"/>
       <c r="G163" s="17" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H163" s="14"/>
     </row>
     <row r="164" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="13"/>
       <c r="B164" s="11" t="s">
-        <v>164</v>
+        <v>119</v>
       </c>
       <c r="C164" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="D164" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="E164" s="35" t="s">
-        <v>13</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="D164" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="E164" s="11"/>
       <c r="F164" s="11"/>
       <c r="G164" s="17" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="H164" s="14"/>
     </row>
     <row r="165" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="13"/>
       <c r="B165" s="11" t="s">
-        <v>167</v>
+        <v>122</v>
       </c>
       <c r="C165" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D165" s="8" t="s">
-        <v>132</v>
+        <v>159</v>
+      </c>
+      <c r="D165" s="19" t="s">
+        <v>145</v>
       </c>
       <c r="E165" s="11"/>
-      <c r="F165" s="18" t="s">
-        <v>13</v>
-      </c>
+      <c r="F165" s="11"/>
       <c r="G165" s="17" t="s">
-        <v>52</v>
+        <v>160</v>
       </c>
       <c r="H165" s="14"/>
     </row>
     <row r="166" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="13"/>
-      <c r="B166" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C166" s="41"/>
-      <c r="D166" s="41"/>
-      <c r="E166" s="41"/>
-      <c r="F166" s="41"/>
-      <c r="G166" s="42"/>
+      <c r="B166" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C166" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D166" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="E166" s="11"/>
+      <c r="F166" s="11"/>
+      <c r="G166" s="17" t="s">
+        <v>163</v>
+      </c>
       <c r="H166" s="14"/>
     </row>
     <row r="167" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="13"/>
-      <c r="B167" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C167" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D167" s="22"/>
-      <c r="E167" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F167" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G167" s="3"/>
+      <c r="B167" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C167" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D167" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E167" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F167" s="11"/>
+      <c r="G167" s="17" t="s">
+        <v>166</v>
+      </c>
       <c r="H167" s="14"/>
     </row>
     <row r="168" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="13"/>
-      <c r="B168" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C168" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D168" s="22"/>
-      <c r="E168" s="8" t="s">
+      <c r="B168" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C168" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="F168" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G168" s="10"/>
+      <c r="D168" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E168" s="11"/>
+      <c r="F168" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G168" s="17" t="s">
+        <v>52</v>
+      </c>
       <c r="H168" s="14"/>
     </row>
     <row r="169" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="13"/>
-      <c r="B169" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C169" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="D169" s="22"/>
-      <c r="E169" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="F169" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="G169" s="10"/>
+      <c r="B169" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C169" s="31"/>
+      <c r="D169" s="31"/>
+      <c r="E169" s="31"/>
+      <c r="F169" s="31"/>
+      <c r="G169" s="32"/>
       <c r="H169" s="14"/>
     </row>
     <row r="170" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="13"/>
-      <c r="B170" s="16" t="s">
+      <c r="B170" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C170" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D170" s="29"/>
+      <c r="E170" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G170" s="3"/>
+      <c r="H170" s="14"/>
+    </row>
+    <row r="171" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="13"/>
+      <c r="B171" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C171" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D171" s="29"/>
+      <c r="E171" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F171" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G171" s="10"/>
+      <c r="H171" s="14"/>
+    </row>
+    <row r="172" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="13"/>
+      <c r="B172" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C170" s="21" t="s">
+      <c r="C172" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D172" s="29"/>
+      <c r="E172" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="F172" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G172" s="10"/>
+      <c r="H172" s="14"/>
+    </row>
+    <row r="173" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="13"/>
+      <c r="B173" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C173" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="D170" s="22"/>
-      <c r="E170" s="40" t="s">
+      <c r="D173" s="29"/>
+      <c r="E173" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="F170" s="40" t="s">
+      <c r="F173" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="G170" s="10"/>
-      <c r="H170" s="14"/>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A171" s="20"/>
-      <c r="B171" s="1"/>
-      <c r="C171" s="1"/>
-      <c r="D171" s="1"/>
-      <c r="E171" s="1"/>
-      <c r="F171" s="1"/>
-      <c r="G171" s="1"/>
-      <c r="H171" s="20"/>
-    </row>
-    <row r="172" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="173" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="174" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="G173" s="10"/>
+      <c r="H173" s="14"/>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A174" s="20"/>
+      <c r="B174" s="1"/>
+      <c r="C174" s="1"/>
+      <c r="D174" s="1"/>
+      <c r="E174" s="1"/>
+      <c r="F174" s="1"/>
+      <c r="G174" s="1"/>
+      <c r="H174" s="20"/>
+    </row>
     <row r="175" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="176" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4751,78 +4817,81 @@
     <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="B140:G140"/>
-    <mergeCell ref="B128:G128"/>
-    <mergeCell ref="B127:G127"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="C167:D167"/>
-    <mergeCell ref="C168:D168"/>
-    <mergeCell ref="C169:D169"/>
-    <mergeCell ref="C170:D170"/>
-    <mergeCell ref="C141:D141"/>
-    <mergeCell ref="C142:D142"/>
-    <mergeCell ref="C143:D143"/>
-    <mergeCell ref="B145:G145"/>
-    <mergeCell ref="B146:G146"/>
-    <mergeCell ref="B166:G166"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="B73:G73"/>
-    <mergeCell ref="B81:G81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="B61:G61"/>
-    <mergeCell ref="B62:G62"/>
-    <mergeCell ref="B68:G68"/>
-    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="B105:G105"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="B89:G89"/>
+    <mergeCell ref="B90:G90"/>
+    <mergeCell ref="B100:G100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
     <mergeCell ref="B49:G49"/>
     <mergeCell ref="B50:G50"/>
     <mergeCell ref="B56:G56"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="C58:D58"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="B61:G61"/>
+    <mergeCell ref="B62:G62"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="B73:G73"/>
+    <mergeCell ref="B74:G74"/>
+    <mergeCell ref="B84:G84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C170:D170"/>
+    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="C172:D172"/>
+    <mergeCell ref="C173:D173"/>
+    <mergeCell ref="C144:D144"/>
+    <mergeCell ref="C145:D145"/>
+    <mergeCell ref="C146:D146"/>
+    <mergeCell ref="B148:G148"/>
+    <mergeCell ref="B149:G149"/>
+    <mergeCell ref="B169:G169"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="B143:G143"/>
+    <mergeCell ref="B131:G131"/>
+    <mergeCell ref="B130:G130"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="C126:D126"/>
     <mergeCell ref="C125:D125"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="B102:G102"/>
-    <mergeCell ref="B103:G103"/>
-    <mergeCell ref="B121:G121"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="B86:G86"/>
-    <mergeCell ref="B87:G87"/>
-    <mergeCell ref="B97:G97"/>
-    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="B106:G106"/>
+    <mergeCell ref="B124:G124"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>